<commit_message>
Deploying to gh-pages from  @ 2c8273737a436af4ee6c2d0f99e29d7e787d77ad 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2023_6-1-1.xlsx
+++ b/assets/excel/2023_6-1-1.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15_Uebergreifende_Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D0DC1E-E9AE-4450-BFE5-68B8E87E1546}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC24E29C-5855-4DF4-B02B-581513F44C04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{AA243A32-41BB-4F7E-BF62-306402113A43}"/>
   </bookViews>
@@ -323,33 +323,11 @@
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -357,18 +335,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -405,22 +371,56 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -447,7 +447,7 @@
     <sheetNames>
       <sheetName val="2022_Downloadtabelle"/>
       <sheetName val="6_1_1_CSV_Vorbereitung"/>
-      <sheetName val="6-1-1_CDV_Export"/>
+      <sheetName val="6-1-1_CSV_Export"/>
       <sheetName val="2022_Bund"/>
       <sheetName val="2022_Land"/>
       <sheetName val="2021_Bund"/>
@@ -965,9 +965,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EFB8D67-ECFF-4568-983A-C81D8BF3E048}">
+  <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:R31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -983,949 +986,955 @@
     </row>
     <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
     </row>
     <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="9"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="35"/>
     </row>
     <row r="7" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12">
+      <c r="B7" s="29"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="5">
         <v>2005</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="5">
         <v>2007</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="5">
         <v>2009</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="5">
         <v>2010</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="5">
         <v>2012</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="5">
         <v>2013</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="5">
         <v>2014</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="5">
         <v>2015</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="5">
         <v>2016</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="5">
         <v>2017</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="6">
         <v>2018</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="6">
         <v>2019</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="6">
         <v>2020</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="6">
         <v>2021</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7" s="7">
         <v>2022</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="18"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="37"/>
     </row>
     <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19">
+      <c r="B9" s="8">
         <v>1</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="8">
         <v>2</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="8">
         <v>3</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="8">
         <v>4</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="8">
         <v>5</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="8">
         <v>6</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="8">
         <v>7</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="8">
         <v>8</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="8">
         <v>9</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="8">
         <v>10</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="8">
         <v>11</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="8">
         <v>12</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="9">
         <v>13</v>
       </c>
-      <c r="O9" s="20">
+      <c r="O9" s="9">
         <v>14</v>
       </c>
-      <c r="P9" s="20">
+      <c r="P9" s="9">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="11">
         <v>13.1</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="11">
         <v>12.8</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="11">
         <v>13</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="11">
         <v>12.9</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="11">
         <v>13.9</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="11">
         <v>14.5</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="11">
         <v>13.8</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="11">
         <v>14</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="11">
         <v>13.5</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="11">
         <v>13.3</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="12">
         <v>12.5</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="12">
         <f>'[1]2019_A3.9 NI_Land'!P55</f>
         <v>13.4</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="12">
         <f>'[1]2022_Land'!B55</f>
         <v>14</v>
       </c>
-      <c r="Q10" s="23">
+      <c r="Q10" s="12">
         <f>'[1]2021_A3.9 NI_LAND'!C55</f>
         <v>14.4</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="12">
         <f>'[1]2022_Land'!D55</f>
         <v>14.1</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="11">
         <v>43</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="11">
         <v>40.299999999999997</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="11">
         <v>37.9</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="11">
         <v>36.700000000000003</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="11">
         <v>36.5</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="11">
         <v>36</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="11">
         <v>36.6</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="11">
         <v>40.5</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="11">
         <v>43</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="11">
         <v>41</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="12">
         <v>38.5</v>
       </c>
-      <c r="O11" s="23">
+      <c r="O11" s="12">
         <f>'[1]2019_A3.9 NI_Land'!P54</f>
         <v>40.799999999999997</v>
       </c>
-      <c r="P11" s="23">
+      <c r="P11" s="12">
         <f>'[1]2022_Land'!B54</f>
         <v>43.7</v>
       </c>
-      <c r="Q11" s="23">
+      <c r="Q11" s="12">
         <f>'[1]2021_A3.9 NI_LAND'!C54</f>
         <v>41.2</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="12">
         <f>'[1]2022_Land'!D54</f>
         <v>40.6</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="11">
         <v>33.200000000000003</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="11">
         <v>32.200000000000003</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="11">
         <v>29.7</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="11">
         <v>29.1</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="11">
         <v>28.7</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="11">
         <v>28.5</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="11">
         <v>27.7</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="11">
         <v>30.2</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="11">
         <v>30.9</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="11">
         <v>30.1</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="12">
         <v>28.2</v>
       </c>
-      <c r="O12" s="23">
+      <c r="O12" s="12">
         <f>'[1]2019_A3.9 NI_Land'!P57</f>
         <v>30.4</v>
       </c>
-      <c r="P12" s="23">
+      <c r="P12" s="12">
         <f>'[1]2022_Land'!B57</f>
         <v>32.1</v>
       </c>
-      <c r="Q12" s="23">
+      <c r="Q12" s="12">
         <f>'[1]2021_A3.9 NI_LAND'!C57</f>
         <v>30.1</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="12">
         <f>'[1]2022_Land'!D57</f>
         <v>30.4</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="11">
         <v>11.7</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="11">
         <v>11.3</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="11">
         <v>11.5</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="11">
         <v>11.5</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="11">
         <v>12.4</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="11">
         <v>13</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="11">
         <v>12.6</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="11">
         <v>12.7</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="11">
         <v>12.2</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="11">
         <v>11.9</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="12">
         <v>11.2</v>
       </c>
-      <c r="O13" s="23">
+      <c r="O13" s="12">
         <f>'[1]2019_A3.9 NI_Land'!P58</f>
         <v>11.9</v>
       </c>
-      <c r="P13" s="23">
+      <c r="P13" s="12">
         <f>'[1]2022_Land'!B58</f>
         <v>12.5</v>
       </c>
-      <c r="Q13" s="23">
+      <c r="Q13" s="12">
         <f>'[1]2021_A3.9 NI_LAND'!C58</f>
         <v>13</v>
       </c>
-      <c r="R13" s="23">
+      <c r="R13" s="12">
         <f>'[1]2022_Land'!D58</f>
         <v>12.6</v>
       </c>
     </row>
-    <row r="14" spans="2:18" s="27" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
+    <row r="14" spans="2:18" s="16" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="14">
         <v>15.1</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="14">
         <v>14.7</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="14">
         <v>14.6</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="14">
         <v>14.5</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="14">
         <v>15.2</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="14">
         <v>15.8</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="14">
         <v>15.3</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="14">
         <v>15.9</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="14">
         <v>16</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="14">
         <v>15.8</v>
       </c>
-      <c r="N14" s="26">
+      <c r="N14" s="15">
         <v>15</v>
       </c>
-      <c r="O14" s="26">
+      <c r="O14" s="15">
         <f>'[1]2019_A3.9 NI_Land'!P6</f>
         <v>16</v>
       </c>
-      <c r="P14" s="26">
+      <c r="P14" s="15">
         <f>'[1]2022_Land'!B6</f>
         <v>17</v>
       </c>
-      <c r="Q14" s="26">
+      <c r="Q14" s="15">
         <f>'[1]2021_A3.9 NI_LAND'!C6</f>
         <v>17.100000000000001</v>
       </c>
-      <c r="R14" s="26">
+      <c r="R14" s="15">
         <f>'[1]2022_Land'!D6</f>
         <v>17.100000000000001</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="11">
         <v>12.8</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="11">
         <v>12.5</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="11">
         <v>13</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="11">
         <v>12.9</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="11">
         <v>13.6</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="11">
         <v>13.9</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="11">
         <v>13.7</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="11">
         <v>13.8</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="11">
         <v>13.3</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="11">
         <v>13.1</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="12">
         <v>12.8</v>
       </c>
-      <c r="O15" s="23">
+      <c r="O15" s="12">
         <f>'[1]2019_A2.0 DE_Bund'!P55</f>
         <v>13.2</v>
       </c>
-      <c r="P15" s="23">
+      <c r="P15" s="12">
         <f>'[1]2022_Bund'!B55</f>
         <v>13.3</v>
       </c>
-      <c r="Q15" s="23">
+      <c r="Q15" s="12">
         <f>'[1]2021_Bund'!C55</f>
         <v>14.1</v>
       </c>
-      <c r="R15" s="23">
+      <c r="R15" s="12">
         <f>'[1]2022_Bund'!D55</f>
         <v>13.7</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="11">
         <v>34.299999999999997</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="11">
         <v>32.6</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="11">
         <v>31.8</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="11">
         <v>31.7</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="11">
         <v>31.5</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="11">
         <v>32</v>
       </c>
-      <c r="J16" s="22">
+      <c r="J16" s="11">
         <v>32.5</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="11">
         <v>33.700000000000003</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="11">
         <v>35.5</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="11">
         <v>36.200000000000003</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="12">
         <v>34.799999999999997</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O16" s="12">
         <f>'[1]2019_A2.0 DE_Bund'!P54</f>
         <v>35.200000000000003</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P16" s="12">
         <f>'[1]2022_Bund'!B54</f>
         <v>35.9</v>
       </c>
-      <c r="Q16" s="23">
+      <c r="Q16" s="12">
         <f>'[1]2021_Bund'!C54</f>
         <v>35.9</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="12">
         <f>'[1]2022_Bund'!D54</f>
         <v>35.299999999999997</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="11">
         <v>28.2</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="11">
         <v>26.9</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="11">
         <v>26.6</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="11">
         <v>26.2</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="11">
         <v>26.3</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="11">
         <v>26.6</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="11">
         <v>26.7</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="11">
         <v>27.7</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="11">
         <v>28</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="11">
         <v>28.6</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="12">
         <v>27.2</v>
       </c>
-      <c r="O17" s="23">
+      <c r="O17" s="12">
         <f>'[1]2019_A2.0 DE_Bund'!P57</f>
         <v>27.8</v>
       </c>
-      <c r="P17" s="23">
+      <c r="P17" s="12">
         <f>'[1]2022_Bund'!B57</f>
         <v>28</v>
       </c>
-      <c r="Q17" s="23">
+      <c r="Q17" s="12">
         <f>'[1]2021_Bund'!C57</f>
         <v>28.6</v>
       </c>
-      <c r="R17" s="23">
+      <c r="R17" s="12">
         <f>'[1]2022_Bund'!D57</f>
         <v>28.1</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="11">
         <v>11.6</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="11">
         <v>11.3</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="11">
         <v>11.7</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="11">
         <v>11.7</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="11">
         <v>12.3</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="11">
         <v>12.6</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="11">
         <v>12.5</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="11">
         <v>12.5</v>
       </c>
-      <c r="L18" s="22">
+      <c r="L18" s="11">
         <v>12.1</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="11">
         <v>11.8</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N18" s="12">
         <v>11.4</v>
       </c>
-      <c r="O18" s="23">
+      <c r="O18" s="12">
         <f>'[1]2019_A2.0 DE_Bund'!P58</f>
         <v>11.7</v>
       </c>
-      <c r="P18" s="23">
+      <c r="P18" s="12">
         <f>'[1]2022_Bund'!B58</f>
         <v>11.8</v>
       </c>
-      <c r="Q18" s="23">
+      <c r="Q18" s="12">
         <f>'[1]2021_Bund'!C58</f>
         <v>12.5</v>
       </c>
-      <c r="R18" s="23">
+      <c r="R18" s="12">
         <f>'[1]2022_Bund'!D58</f>
         <v>12.1</v>
       </c>
     </row>
-    <row r="19" spans="2:18" s="27" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="24" t="s">
+    <row r="19" spans="2:18" s="16" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="14">
         <v>14.7</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="14">
         <v>14.3</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="14">
         <v>14.6</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="14">
         <v>14.5</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="14">
         <v>15</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="14">
         <v>15.5</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="14">
         <v>15.4</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="14">
         <v>15.7</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="14">
         <v>15.7</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="14">
         <v>15.8</v>
       </c>
-      <c r="N19" s="26">
+      <c r="N19" s="15">
         <v>15.5</v>
       </c>
-      <c r="O19" s="26">
+      <c r="O19" s="15">
         <f>'[1]2019_A2.0 DE_Bund'!P6</f>
         <v>15.9</v>
       </c>
-      <c r="P19" s="26">
+      <c r="P19" s="15">
         <f>'[1]2022_Bund'!B6</f>
         <v>16.2</v>
       </c>
-      <c r="Q19" s="26">
+      <c r="Q19" s="15">
         <f>'[1]2021_Bund'!C6</f>
         <v>16.899999999999999</v>
       </c>
-      <c r="R19" s="26">
+      <c r="R19" s="15">
         <f>'[1]2022_Bund'!D6</f>
         <v>16.7</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
     </row>
     <row r="21" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
     </row>
     <row r="22" spans="2:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
     </row>
     <row r="24" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
     </row>
     <row r="25" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
     </row>
     <row r="26" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
     </row>
     <row r="27" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
     </row>
     <row r="28" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
     </row>
     <row r="29" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="34"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
     </row>
     <row r="30" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
     </row>
     <row r="31" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:R6"/>
+    <mergeCell ref="D8:R8"/>
     <mergeCell ref="B29:M29"/>
     <mergeCell ref="B30:M30"/>
     <mergeCell ref="B31:M31"/>
@@ -1935,12 +1944,6 @@
     <mergeCell ref="B26:M26"/>
     <mergeCell ref="B27:M27"/>
     <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:R6"/>
-    <mergeCell ref="D8:R8"/>
-    <mergeCell ref="B21:M21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B31" r:id="rId1" xr:uid="{5648539E-0E7E-4489-8DA0-DBE6BB9388F9}"/>

</xml_diff>